<commit_message>
create a new table named immu_knowledge
</commit_message>
<xml_diff>
--- a/database_draft.xlsx
+++ b/database_draft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="加拿大健康安全新闻" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve"> id</t>
-  </si>
-  <si>
-    <t>importance</t>
   </si>
   <si>
     <t>immu_times</t>
@@ -246,10 +243,6 @@
     <t>news_immunized_2.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-IPV-Hib or DTaP-HB-IPV-Hib
-</t>
-  </si>
-  <si>
     <t>Diphtheria, Tetanus, acellular Pertussis, Polio and Haemophilus influenzae type b (DTaP-IPV-Hib) is a combined vaccine that protects children against five diseases ― diphtheria, tetanus, pertussis, polio and serious diseases like meningitis caused by the Hib (Haemophilus influenzae type b) germ.  The abbreviation "aP" stands for "acellular pertussis." Hib vaccine is also available as a separate shot.</t>
   </si>
   <si>
@@ -294,86 +287,92 @@
     <t>Measles causes fever, rash, cough, and runny nose, and red, watery eyes. Complications can include ear infection, diarrhea, pneumonia, brain damage, and death. Mumps causes fever, headache, muscle aches, tiredness, loss of appetite, and swollen salivary glands. Complications can include swelling of the testicles or ovaries, deafness, inflammation of the. Rubella causes fever, sore throat, rash, headache, and red, itchy eyesVaricella (chickenpox) causes blister-like rash, itching, fever, and tiredness. Complications can include severe skin infection, scars, pneumo¬nia, brain damage, or death.</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-IPV  or Tdap-IPV
+    <t>TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.</t>
+  </si>
+  <si>
+    <t>HB</t>
+  </si>
+  <si>
+    <t>Hepatitis B is an infectious disease caused by the hepatitis B virus (HBV) which affects the liver. It can cause both acute and chronic infections. Many people have no symptoms during the initial infection. Some develop a rapid onset of sickness with vomiting, yellowish skin, tiredness, dark urine and abdominal pain. Often these symptoms last a few weeks and rarely does the initial infection result in death. It may take 30 to 180 days for symptoms to begin. Most of those with chronic disease have no symptoms; however, cirrhosis and liver cancer may eventually develop.</t>
+  </si>
+  <si>
+    <t>Men-C-ACYW135</t>
+  </si>
+  <si>
+    <t>Men-C-ACYW-135-CRM contains capsular polysaccharides from serogroups A (10 μg), C (5 μg), W135 (5 μg) and Y (5 μg). The vaccine contains no adjuvant, preservatives, or thimerosal. The container closures do not contain latex. The vaccine is packaged in two separate vials that are mixed prior to administration. Subsequently, 0.5 ml of the reconstituted solution is withdrawn from the vial that previously contained the meningococcal A powder. There may be a small amount of reconstituted vaccine remaining in the vial after the 0.5 ml is withdrawn.</t>
+  </si>
+  <si>
+    <t>HPV</t>
+  </si>
+  <si>
+    <t>HPV is the most common sexually transmitted infection (STI). HPV is a different virus than HIV and HSV (herpes). HPV is so common that nearly all sexually active men and women get it at some point in their lives. There are many different types of HPV. Some types can cause health problems including genital warts and cancers. But there are vaccines that can stop these health problems from happening.</t>
+  </si>
+  <si>
+    <t>Tdap</t>
+  </si>
+  <si>
+    <t>Tdap is a combination vaccine that protects against three potentially life-threatening bacterial diseases: tetanus, diphtheria, and pertussis (whooping cough). Td is a booster vaccine for tetanus and diphtheria. It does not protect against pertussis.</t>
+  </si>
+  <si>
+    <t>Hib</t>
+  </si>
+  <si>
+    <t>Haemophilus influenzae type B vaccine is a vaccine used to prevent Haemophilus influenzae type b infection. In countries that include it as a routine vaccine, rates of severe Hib infections have decreased more than 90%</t>
+  </si>
+  <si>
+    <t>Pneu-P-23</t>
+  </si>
+  <si>
+    <t>Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. When you are immunized, you also help protect others because you are less likely to spread infection.</t>
+  </si>
+  <si>
+    <t>4CMenB</t>
+  </si>
+  <si>
+    <t>The 4CMenB vaccine is an immunogenic vaccine, though its effectiveness, impact on carriage and the duration of protection remains unknown. Further research, evaluation and surveillance will be required to determine the duration of protection, the efficacy or effectiveness of 4CMenB vaccine, its ability to induce herd protection, and the risk of adverse events with widespread use.</t>
+  </si>
+  <si>
+    <t>HA</t>
+  </si>
+  <si>
+    <t>Hepatitis A is an infection of the liver caused by a virus. Adults and children are equally at risk. The virus most frequently spreads through direct contact with infected people or indirectly through ingestion of contaminated foods or water. Symptoms include fever, fatigue, loss of appetite, nausea, vomiting, abdominal pain, and jaundice (yellow skin and eyes).</t>
+  </si>
+  <si>
+    <t>Typh-I</t>
+  </si>
+  <si>
+    <t>Typhoid vaccine can prevent typhoid. There are two vaccines to prevent typhoid. One is an inactivated (killed) vaccine gotten as a shot, and the other is live, attenuated (weakened) vaccine, which is taken orally (by mouth).</t>
+  </si>
+  <si>
+    <t>BCG</t>
+  </si>
+  <si>
+    <t>Bacillus Calmette–Guérin (BCG) vaccine is a vaccine primarily used against tuberculosis. Tuberculosis (TB) is a potentially serious infectious disease that mainly affects your lungs. The bacteria that cause tuberculosis are spread from one person to another through tiny droplets released into the air via coughs and sneezes.</t>
+  </si>
+  <si>
+    <t>2016-2-25</t>
+  </si>
+  <si>
+    <t>2016-2-26</t>
+  </si>
+  <si>
+    <t>2016-2-27</t>
+  </si>
+  <si>
+    <t>2016-2-24</t>
+  </si>
+  <si>
+    <t>2016-1-28</t>
+  </si>
+  <si>
+    <t>immu_importance</t>
+  </si>
+  <si>
+    <t>DTaP-IPV-Hib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTaP-IPV
 </t>
-  </si>
-  <si>
-    <t>TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.</t>
-  </si>
-  <si>
-    <t>HB</t>
-  </si>
-  <si>
-    <t>Hepatitis B is an infectious disease caused by the hepatitis B virus (HBV) which affects the liver. It can cause both acute and chronic infections. Many people have no symptoms during the initial infection. Some develop a rapid onset of sickness with vomiting, yellowish skin, tiredness, dark urine and abdominal pain. Often these symptoms last a few weeks and rarely does the initial infection result in death. It may take 30 to 180 days for symptoms to begin. Most of those with chronic disease have no symptoms; however, cirrhosis and liver cancer may eventually develop.</t>
-  </si>
-  <si>
-    <t>Men-C-ACYW135</t>
-  </si>
-  <si>
-    <t>Men-C-ACYW-135-CRM contains capsular polysaccharides from serogroups A (10 μg), C (5 μg), W135 (5 μg) and Y (5 μg). The vaccine contains no adjuvant, preservatives, or thimerosal. The container closures do not contain latex. The vaccine is packaged in two separate vials that are mixed prior to administration. Subsequently, 0.5 ml of the reconstituted solution is withdrawn from the vial that previously contained the meningococcal A powder. There may be a small amount of reconstituted vaccine remaining in the vial after the 0.5 ml is withdrawn.</t>
-  </si>
-  <si>
-    <t>HPV</t>
-  </si>
-  <si>
-    <t>HPV is the most common sexually transmitted infection (STI). HPV is a different virus than HIV and HSV (herpes). HPV is so common that nearly all sexually active men and women get it at some point in their lives. There are many different types of HPV. Some types can cause health problems including genital warts and cancers. But there are vaccines that can stop these health problems from happening.</t>
-  </si>
-  <si>
-    <t>Tdap</t>
-  </si>
-  <si>
-    <t>Tdap is a combination vaccine that protects against three potentially life-threatening bacterial diseases: tetanus, diphtheria, and pertussis (whooping cough). Td is a booster vaccine for tetanus and diphtheria. It does not protect against pertussis.</t>
-  </si>
-  <si>
-    <t>Hib</t>
-  </si>
-  <si>
-    <t>Haemophilus influenzae type B vaccine is a vaccine used to prevent Haemophilus influenzae type b infection. In countries that include it as a routine vaccine, rates of severe Hib infections have decreased more than 90%</t>
-  </si>
-  <si>
-    <t>Pneu-P-23</t>
-  </si>
-  <si>
-    <t>Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. When you are immunized, you also help protect others because you are less likely to spread infection.</t>
-  </si>
-  <si>
-    <t>4CMenB</t>
-  </si>
-  <si>
-    <t>The 4CMenB vaccine is an immunogenic vaccine, though its effectiveness, impact on carriage and the duration of protection remains unknown. Further research, evaluation and surveillance will be required to determine the duration of protection, the efficacy or effectiveness of 4CMenB vaccine, its ability to induce herd protection, and the risk of adverse events with widespread use.</t>
-  </si>
-  <si>
-    <t>HA</t>
-  </si>
-  <si>
-    <t>Hepatitis A is an infection of the liver caused by a virus. Adults and children are equally at risk. The virus most frequently spreads through direct contact with infected people or indirectly through ingestion of contaminated foods or water. Symptoms include fever, fatigue, loss of appetite, nausea, vomiting, abdominal pain, and jaundice (yellow skin and eyes).</t>
-  </si>
-  <si>
-    <t>Typh-I</t>
-  </si>
-  <si>
-    <t>Typhoid vaccine can prevent typhoid. There are two vaccines to prevent typhoid. One is an inactivated (killed) vaccine gotten as a shot, and the other is live, attenuated (weakened) vaccine, which is taken orally (by mouth).</t>
-  </si>
-  <si>
-    <t>BCG</t>
-  </si>
-  <si>
-    <t>Bacillus Calmette–Guérin (BCG) vaccine is a vaccine primarily used against tuberculosis. Tuberculosis (TB) is a potentially serious infectious disease that mainly affects your lungs. The bacteria that cause tuberculosis are spread from one person to another through tiny droplets released into the air via coughs and sneezes.</t>
-  </si>
-  <si>
-    <t>2016-2-25</t>
-  </si>
-  <si>
-    <t>2016-2-26</t>
-  </si>
-  <si>
-    <t>2016-2-27</t>
-  </si>
-  <si>
-    <t>2016-2-24</t>
-  </si>
-  <si>
-    <t>2016-1-28</t>
   </si>
 </sst>
 </file>
@@ -804,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="379.9" customHeight="1">
@@ -812,22 +811,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="379.9" customHeight="1">
@@ -835,22 +834,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="379.9" customHeight="1">
@@ -858,22 +857,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1003,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1037,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="282.60000000000002" customHeight="1">
@@ -1045,22 +1044,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.5">
@@ -1068,22 +1067,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="270">
@@ -1091,22 +1090,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1198,21 +1197,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1223,389 +1223,467 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="181.9" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="181.9" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="5">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="255">
+      <c r="F2" t="str">
+        <f>CONCATENATE("(",A2,",'",B2,"','",C2,"',",D2,",",E2,")",",")</f>
+        <v>(1,'DTaP-IPV-Hib','Diphtheria, Tetanus, acellular Pertussis, Polio and Haemophilus influenzae type b (DTaP-IPV-Hib) is a combined vaccine that protects children against five diseases ― diphtheria, tetanus, pertussis, polio and serious diseases like meningitis caused by the Hib (Haemophilus influenzae type b) germ.  The abbreviation "aP" stands for "acellular pertussis." Hib vaccine is also available as a separate shot.',4,1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="5">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="195">
+      <c r="F3" t="str">
+        <f>CONCATENATE("(",A3,",'",B3,"','",C3,"',",D3,",",E3,")",",")</f>
+        <v>(2,'Pneu-C-13','Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. There are more than 90 different types of pneumococcal bacteria. Pneu-C-13 vaccine protects against the l3 types that cause most of the severe pneumococcal infections in children.',3,1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="105">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="5">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="E4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="210">
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F19" si="0">CONCATENATE("(",A4,",'",B4,"','",C4,"',",D4,",",E4,")",",")</f>
+        <v>(3,'Rot','Rotavirus is the most common cause of severe vomiting and diarrhoea among infants and young children。 It is a genus of double-stranded RNA virus in the family Reoviridae. Nearly every child in the world has been infected with rotavirus at least once by the age of five.  Immunity develops with each infection, so subsequent infections are less severe; adults are rarely affected。 ',2,1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="120">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="5">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="180">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,'MMR','The MMR vaccine protects against measles, mumps, and rubella. The vaccine contains weakened forms of the measles, mumps and rubella viruses that do not cause disease. The vaccine is approved by Health Canada.
+The MMR vaccine is provided free as part of your child’s routine immunizations. Call your health care provider to make an appointment.
+',2,1),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="270">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,'Men-C-C','The Men-C vaccine protects against infection from one of the most common types of meningococcal bacteria, type C. The vaccine is approved by Health Canada.
+The Men-C vaccine is provided free as part of your child’s routine immunizations. Call your health care provider to make an appointment.
+',1,1),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="135">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="5">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="330">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,'MMR  and Var
+','Varicella, also known as chickenpox, is a very common and highly infectious childhood disease that is found worldwide. Symptoms appear 10 to 21 days after infection and last about 2 weeks. The defining symptom is a characteristic blister-like rash, which can cause severe irritation. Most children have a relatively mild illness, but severe illness may occur in adults and people with depressed immunity because of existing illness or because of a treatment that they are receiving',2,1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="180">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="5">
+        <v>53</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="5">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="E8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="315">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,'MMRV','Measles causes fever, rash, cough, and runny nose, and red, watery eyes. Complications can include ear infection, diarrhea, pneumonia, brain damage, and death. Mumps causes fever, headache, muscle aches, tiredness, loss of appetite, and swollen salivary glands. Complications can include swelling of the testicles or ovaries, deafness, inflammation of the. Rubella causes fever, sore throat, rash, headache, and red, itchy eyesVaricella (chickenpox) causes blister-like rash, itching, fever, and tiredness. Complications can include severe skin infection, scars, pneumo¬nia, brain damage, or death.',2,1),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="180">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>58</v>
+        <v>83</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="300">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,'DTaP-IPV
+','TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.',1,1),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="165">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="5">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E10" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="285">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,'HB','Hepatitis B is an infectious disease caused by the hepatitis B virus (HBV) which affects the liver. It can cause both acute and chronic infections. Many people have no symptoms during the initial infection. Some develop a rapid onset of sickness with vomiting, yellowish skin, tiredness, dark urine and abdominal pain. Often these symptoms last a few weeks and rarely does the initial infection result in death. It may take 30 to 180 days for symptoms to begin. Most of those with chronic disease have no symptoms; however, cirrhosis and liver cancer may eventually develop.',2,1),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="165">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
       </c>
       <c r="E11" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="225">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,'Men-C-ACYW135','Men-C-ACYW-135-CRM contains capsular polysaccharides from serogroups A (10 μg), C (5 μg), W135 (5 μg) and Y (5 μg). The vaccine contains no adjuvant, preservatives, or thimerosal. The container closures do not contain latex. The vaccine is packaged in two separate vials that are mixed prior to administration. Subsequently, 0.5 ml of the reconstituted solution is withdrawn from the vial that previously contained the meningococcal A powder. There may be a small amount of reconstituted vaccine remaining in the vial after the 0.5 ml is withdrawn.',1,1),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="120">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="5">
+        <v>60</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="5">
         <v>2</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="E12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="135">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,'HPV','HPV is the most common sexually transmitted infection (STI). HPV is a different virus than HIV and HSV (herpes). HPV is so common that nearly all sexually active men and women get it at some point in their lives. There are many different types of HPV. Some types can cause health problems including genital warts and cancers. But there are vaccines that can stop these health problems from happening.',2,1),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="75">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
       </c>
       <c r="E13" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="120">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,'Tdap','Tdap is a combination vaccine that protects against three potentially life-threatening bacterial diseases: tetanus, diphtheria, and pertussis (whooping cough). Td is a booster vaccine for tetanus and diphtheria. It does not protect against pertussis.',1,1),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="210">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,'Hib','Haemophilus influenzae type B vaccine is a vaccine used to prevent Haemophilus influenzae type b infection. In countries that include it as a routine vaccine, rates of severe Hib infections have decreased more than 90%',1,0),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="105">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="210">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,'Pneu-P-23','Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. When you are immunized, you also help protect others because you are less likely to spread infection.',1,0),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="120">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="5">
+        <v>68</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="5">
         <v>3</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="195">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,'4CMenB','The 4CMenB vaccine is an immunogenic vaccine, though its effectiveness, impact on carriage and the duration of protection remains unknown. Further research, evaluation and surveillance will be required to determine the duration of protection, the efficacy or effectiveness of 4CMenB vaccine, its ability to induce herd protection, and the risk of adverse events with widespread use.',3,1),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="105">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="5">
+        <v>70</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="5">
         <v>2</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="150.75" thickBot="1">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,'HA','Hepatitis A is an infection of the liver caused by a virus. Adults and children are equally at risk. The virus most frequently spreads through direct contact with infected people or indirectly through ingestion of contaminated foods or water. Symptoms include fever, fatigue, loss of appetite, nausea, vomiting, abdominal pain, and jaundice (yellow skin and eyes).',2,0),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="75.75" thickBot="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="5">
+        <v>72</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="5">
         <v>3</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="180.75" thickBot="1">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,'Typh-I','Typhoid vaccine can prevent typhoid. There are two vaccines to prevent typhoid. One is an inactivated (killed) vaccine gotten as a shot, and the other is live, attenuated (weakened) vaccine, which is taken orally (by mouth).',3,0),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90.75" thickBot="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,'BCG','Bacillus Calmette–Guérin (BCG) vaccine is a vaccine primarily used against tuberculosis. Tuberculosis (TB) is a potentially serious infectious disease that mainly affects your lungs. The bacteria that cause tuberculosis are spread from one person to another through tiny droplets released into the air via coughs and sneezes.',1,0),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>

</xml_diff>

<commit_message>
fix blank lines in records table
</commit_message>
<xml_diff>
--- a/database_draft.xlsx
+++ b/database_draft.xlsx
@@ -274,10 +274,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">MMR  and Var
-</t>
-  </si>
-  <si>
     <t>Varicella, also known as chickenpox, is a very common and highly infectious childhood disease that is found worldwide. Symptoms appear 10 to 21 days after infection and last about 2 weeks. The defining symptom is a characteristic blister-like rash, which can cause severe irritation. Most children have a relatively mild illness, but severe illness may occur in adults and people with depressed immunity because of existing illness or because of a treatment that they are receiving</t>
   </si>
   <si>
@@ -371,8 +367,10 @@
     <t>DTaP-IPV-Hib</t>
   </si>
   <si>
-    <t xml:space="preserve">DTaP-IPV
-</t>
+    <t>MMR  and Var</t>
+  </si>
+  <si>
+    <t>DTaP-IPV</t>
   </si>
 </sst>
 </file>
@@ -811,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -834,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -857,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
@@ -1044,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
@@ -1067,7 +1065,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>28</v>
@@ -1090,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
@@ -1199,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1226,7 +1224,7 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="181.9" customHeight="1">
@@ -1234,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>42</v>
@@ -1343,10 +1341,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="D7" s="5">
         <v>2</v>
@@ -1356,8 +1354,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>(6,'MMR  and Var
-','Varicella, also known as chickenpox, is a very common and highly infectious childhood disease that is found worldwide. Symptoms appear 10 to 21 days after infection and last about 2 weeks. The defining symptom is a characteristic blister-like rash, which can cause severe irritation. Most children have a relatively mild illness, but severe illness may occur in adults and people with depressed immunity because of existing illness or because of a treatment that they are receiving',2,1),</v>
+        <v>(6,'MMR  and Var','Varicella, also known as chickenpox, is a very common and highly infectious childhood disease that is found worldwide. Symptoms appear 10 to 21 days after infection and last about 2 weeks. The defining symptom is a characteristic blister-like rash, which can cause severe irritation. Most children have a relatively mild illness, but severe illness may occur in adults and people with depressed immunity because of existing illness or because of a treatment that they are receiving',2,1),</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="180">
@@ -1365,10 +1362,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="D8" s="5">
         <v>2</v>
@@ -1389,7 +1386,7 @@
         <v>83</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
@@ -1399,8 +1396,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>(8,'DTaP-IPV
-','TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.',1,1),</v>
+        <v>(8,'DTaP-IPV','TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.',1,1),</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="165">
@@ -1408,10 +1404,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="D10" s="5">
         <v>2</v>
@@ -1429,10 +1425,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -1450,10 +1446,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="D12" s="5">
         <v>2</v>
@@ -1471,10 +1467,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -1492,10 +1488,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -1513,10 +1509,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -1534,10 +1530,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="D16" s="5">
         <v>3</v>
@@ -1555,10 +1551,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="D17" s="5">
         <v>2</v>
@@ -1576,10 +1572,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>73</v>
       </c>
       <c r="D18" s="5">
         <v>3</v>
@@ -1597,10 +1593,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
do some changes for records table
</commit_message>
<xml_diff>
--- a/database_draft.xlsx
+++ b/database_draft.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
   <si>
     <t>id</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Rot</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotavirus is the most common cause of severe vomiting and diarrhoea among infants and young children。 It is a genus of double-stranded RNA virus in the family Reoviridae. Nearly every child in the world has been infected with rotavirus at least once by the age of five.  Immunity develops with each infection, so subsequent infections are less severe; adults are rarely affected。 </t>
-  </si>
-  <si>
     <t>MMR</t>
   </si>
   <si>
@@ -371,19 +368,86 @@
   </si>
   <si>
     <t>DTaP-IPV</t>
+  </si>
+  <si>
+    <t>immu_subtitle</t>
+  </si>
+  <si>
+    <t>Diphtheria, Tetanus, acellular Pertussis, Polio and Haemophilus influenzae type b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotavirus is the most common cause of severe vomiting and diarrhoea among infants and young children. It is a genus of double-stranded RNA virus in the family Reoviridae. Nearly every child in the world has been infected with rotavirus at least once by the age of five.  Immunity develops with each infection, so subsequent infections are less severe; adults are rarely affected。 </t>
+  </si>
+  <si>
+    <t>Rotavirus is the most common cause of severe vomiting and diarrhoea</t>
+  </si>
+  <si>
+    <t>The MMR vaccine protects against measles, mumps, and rubella</t>
+  </si>
+  <si>
+    <t>Against infection from common types of meningococcal bacteria, type C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varicella is a very common and highly infectious childhood disease </t>
+  </si>
+  <si>
+    <t>Measles causes fever, rash, cough, and runny nose</t>
+  </si>
+  <si>
+    <t>Combined vaccine that protects children against diphtheria, tetanus, pertussis and polio</t>
+  </si>
+  <si>
+    <t>Hepatitis B is an infectious disease caused by the hepatitis B virus</t>
+  </si>
+  <si>
+    <t>The vaccine contains no adjuvant, preservatives, or thimerosal</t>
+  </si>
+  <si>
+    <t>HPV is the most common sexually transmitted infection</t>
+  </si>
+  <si>
+    <t>Prevent Haemophilus influenzae type b infection</t>
+  </si>
+  <si>
+    <t>Protects against three diseases: tetanus, diphtheria, and pertussis</t>
+  </si>
+  <si>
+    <t>Pneu-P-23 vaccine efficacy against IPD among the elderly</t>
+  </si>
+  <si>
+    <t>4CMenB antigens are important for meningococcal survival, function, or virulence</t>
+  </si>
+  <si>
+    <t>An infection of the liver caused by a virus</t>
+  </si>
+  <si>
+    <t>Typhoid vaccine can prevent typhoid</t>
+  </si>
+  <si>
+    <t>BCG vaccine is used against tuberculosis</t>
+  </si>
+  <si>
+    <t>Infections of the lungs, blood and covering of the brain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -443,9 +507,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -460,28 +524,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -808,8 +878,8 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>75</v>
+      <c r="B2" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -831,8 +901,8 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>76</v>
+      <c r="B3" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -854,8 +924,8 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>77</v>
+      <c r="B4" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
@@ -875,115 +945,115 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2"/>
-      <c r="B5" s="12"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2"/>
-      <c r="B6" s="12"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
-      <c r="B7" s="12"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2"/>
-      <c r="B8" s="12"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
-      <c r="B9" s="12"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
-      <c r="B10" s="12"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2"/>
-      <c r="B12" s="12"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
-      <c r="B13" s="12"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
-      <c r="B14" s="12"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
-      <c r="B15" s="12"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2"/>
-      <c r="B16" s="12"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2"/>
-      <c r="B19" s="12"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2"/>
-      <c r="B20" s="12"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2"/>
-      <c r="B21" s="12"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2"/>
-      <c r="B22" s="12"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2"/>
-      <c r="B23" s="12"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
@@ -1041,8 +1111,8 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>78</v>
+      <c r="B2" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
@@ -1064,8 +1134,8 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>75</v>
+      <c r="B3" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>28</v>
@@ -1087,8 +1157,8 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>79</v>
+      <c r="B4" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
@@ -1108,7 +1178,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1117,7 +1187,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1126,7 +1196,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1135,7 +1205,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1144,7 +1214,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -1153,7 +1223,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1161,7 +1231,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1169,7 +1239,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1177,7 +1247,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1195,22 +1265,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="96" customWidth="1"/>
+    <col min="2" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="96" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1218,37 +1288,43 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="181.9" customHeight="1">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="181.9" customHeight="1">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="C2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="5">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE("(",A2,",'",B2,"','",C2,"',",D2,",",E2,")",",")</f>
-        <v>(1,'DTaP-IPV-Hib','Diphtheria, Tetanus, acellular Pertussis, Polio and Haemophilus influenzae type b (DTaP-IPV-Hib) is a combined vaccine that protects children against five diseases ― diphtheria, tetanus, pertussis, polio and serious diseases like meningitis caused by the Hib (Haemophilus influenzae type b) germ.  The abbreviation "aP" stands for "acellular pertussis." Hib vaccine is also available as a separate shot.',4,1),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="135">
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE("(",A2,",'",B2,"','",C2,"','",D2,"',",E2,",",F2,")",",")</f>
+        <v>(1,'DTaP-IPV-Hib','Diphtheria, Tetanus, acellular Pertussis, Polio and Haemophilus influenzae type b','Diphtheria, Tetanus, acellular Pertussis, Polio and Haemophilus influenzae type b (DTaP-IPV-Hib) is a combined vaccine that protects children against five diseases ― diphtheria, tetanus, pertussis, polio and serious diseases like meningitis caused by the Hib (Haemophilus influenzae type b) germ.  The abbreviation "aP" stands for "acellular pertussis." Hib vaccine is also available as a separate shot.',4,1),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="135">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1256,20 +1332,23 @@
         <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="5">
+      <c r="E3" s="5">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" t="str">
-        <f>CONCATENATE("(",A3,",'",B3,"','",C3,"',",D3,",",E3,")",",")</f>
-        <v>(2,'Pneu-C-13','Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. There are more than 90 different types of pneumococcal bacteria. Pneu-C-13 vaccine protects against the l3 types that cause most of the severe pneumococcal infections in children.',3,1),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="105">
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G19" si="0">CONCATENATE("(",A3,",'",B3,"','",C3,"','",D3,"',",E3,",",F3,")",",")</f>
+        <v>(2,'Pneu-C-13','Infections of the lungs, blood and covering of the brain','Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. There are more than 90 different types of pneumococcal bacteria. Pneu-C-13 vaccine protects against the l3 types that cause most of the severe pneumococcal infections in children.',3,1),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="105">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1277,413 +1356,472 @@
         <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="5">
+        <v>86</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" ref="F4:F19" si="0">CONCATENATE("(",A4,",'",B4,"','",C4,"',",D4,",",E4,")",",")</f>
-        <v>(3,'Rot','Rotavirus is the most common cause of severe vomiting and diarrhoea among infants and young children。 It is a genus of double-stranded RNA virus in the family Reoviridae. Nearly every child in the world has been infected with rotavirus at least once by the age of five.  Immunity develops with each infection, so subsequent infections are less severe; adults are rarely affected。 ',2,1),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="120">
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'Rot','Rotavirus is the most common cause of severe vomiting and diarrhoea','Rotavirus is the most common cause of severe vomiting and diarrhoea among infants and young children. It is a genus of double-stranded RNA virus in the family Reoviridae. Nearly every child in the world has been infected with rotavirus at least once by the age of five.  Immunity develops with each infection, so subsequent infections are less severe; adults are rarely affected。 ',2,1),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="120">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="E5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="str">
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>(4,'MMR','The MMR vaccine protects against measles, mumps, and rubella. The vaccine contains weakened forms of the measles, mumps and rubella viruses that do not cause disease. The vaccine is approved by Health Canada.
+        <v>(4,'MMR','The MMR vaccine protects against measles, mumps, and rubella','The MMR vaccine protects against measles, mumps, and rubella. The vaccine contains weakened forms of the measles, mumps and rubella viruses that do not cause disease. The vaccine is approved by Health Canada.
 The MMR vaccine is provided free as part of your child’s routine immunizations. Call your health care provider to make an appointment.
 ',2,1),</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="105">
+    <row r="6" spans="1:7" ht="105">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>(5,'Men-C-C','The Men-C vaccine protects against infection from one of the most common types of meningococcal bacteria, type C. The vaccine is approved by Health Canada.
+        <v>(5,'Men-C-C','Against infection from common types of meningococcal bacteria, type C','The Men-C vaccine protects against infection from one of the most common types of meningococcal bacteria, type C. The vaccine is approved by Health Canada.
 The Men-C vaccine is provided free as part of your child’s routine immunizations. Call your health care provider to make an appointment.
 ',1,1),</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="135">
+    <row r="7" spans="1:7" ht="135">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="5">
+        <v>89</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="5">
         <v>2</v>
       </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>(6,'MMR  and Var','Varicella, also known as chickenpox, is a very common and highly infectious childhood disease that is found worldwide. Symptoms appear 10 to 21 days after infection and last about 2 weeks. The defining symptom is a characteristic blister-like rash, which can cause severe irritation. Most children have a relatively mild illness, but severe illness may occur in adults and people with depressed immunity because of existing illness or because of a treatment that they are receiving',2,1),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="180">
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <f>CONCATENATE("(",A7,",'",B7,"','",C7,"','",D7,"',",E7,",",F7,")",",")</f>
+        <v>(6,'MMR  and Var','Varicella is a very common and highly infectious childhood disease ','Varicella, also known as chickenpox, is a very common and highly infectious childhood disease that is found worldwide. Symptoms appear 10 to 21 days after infection and last about 2 weeks. The defining symptom is a characteristic blister-like rash, which can cause severe irritation. Most children have a relatively mild illness, but severe illness may occur in adults and people with depressed immunity because of existing illness or because of a treatment that they are receiving',2,1),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="180">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="E8" s="5">
         <v>2</v>
       </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" t="str">
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>(7,'MMRV','Measles causes fever, rash, cough, and runny nose, and red, watery eyes. Complications can include ear infection, diarrhea, pneumonia, brain damage, and death. Mumps causes fever, headache, muscle aches, tiredness, loss of appetite, and swollen salivary glands. Complications can include swelling of the testicles or ovaries, deafness, inflammation of the. Rubella causes fever, sore throat, rash, headache, and red, itchy eyesVaricella (chickenpox) causes blister-like rash, itching, fever, and tiredness. Complications can include severe skin infection, scars, pneumo¬nia, brain damage, or death.',2,1),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="180">
+        <v>(7,'MMRV','Measles causes fever, rash, cough, and runny nose','Measles causes fever, rash, cough, and runny nose, and red, watery eyes. Complications can include ear infection, diarrhea, pneumonia, brain damage, and death. Mumps causes fever, headache, muscle aches, tiredness, loss of appetite, and swollen salivary glands. Complications can include swelling of the testicles or ovaries, deafness, inflammation of the. Rubella causes fever, sore throat, rash, headache, and red, itchy eyesVaricella (chickenpox) causes blister-like rash, itching, fever, and tiredness. Complications can include severe skin infection, scars, pneumo¬nia, brain damage, or death.',2,1),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="180">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" t="str">
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>(8,'DTaP-IPV','TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.',1,1),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="165">
+        <v>(8,'DTaP-IPV','Combined vaccine that protects children against diphtheria, tetanus, pertussis and polio','TaP-IPV is a combined vaccine that protects children against four diseases ― diphtheria, tetanus, pertussis and polio. The abbreviation "aP" stands for "acellular pertussis." This vaccine is recommended for use in infants and children younger than seven years. Diphtheria is a serious disease of the nose, throat and skin. It causes sore throat, fever and chills. It can be complicated by breathing problems, heart failure and nerve damage. Pertussis can also cause brain damage, seizures and death. Pertussis spreads very easily from an infected person to others through coughing or sneezing.',1,1),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="165">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="E10" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" t="str">
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>(9,'HB','Hepatitis B is an infectious disease caused by the hepatitis B virus (HBV) which affects the liver. It can cause both acute and chronic infections. Many people have no symptoms during the initial infection. Some develop a rapid onset of sickness with vomiting, yellowish skin, tiredness, dark urine and abdominal pain. Often these symptoms last a few weeks and rarely does the initial infection result in death. It may take 30 to 180 days for symptoms to begin. Most of those with chronic disease have no symptoms; however, cirrhosis and liver cancer may eventually develop.',2,1),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="165">
+        <v>(9,'HB','Hepatitis B is an infectious disease caused by the hepatitis B virus','Hepatitis B is an infectious disease caused by the hepatitis B virus (HBV) which affects the liver. It can cause both acute and chronic infections. Many people have no symptoms during the initial infection. Some develop a rapid onset of sickness with vomiting, yellowish skin, tiredness, dark urine and abdominal pain. Often these symptoms last a few weeks and rarely does the initial infection result in death. It may take 30 to 180 days for symptoms to begin. Most of those with chronic disease have no symptoms; however, cirrhosis and liver cancer may eventually develop.',2,1),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="165">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
       <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>(10,'Men-C-ACYW135','Men-C-ACYW-135-CRM contains capsular polysaccharides from serogroups A (10 μg), C (5 μg), W135 (5 μg) and Y (5 μg). The vaccine contains no adjuvant, preservatives, or thimerosal. The container closures do not contain latex. The vaccine is packaged in two separate vials that are mixed prior to administration. Subsequently, 0.5 ml of the reconstituted solution is withdrawn from the vial that previously contained the meningococcal A powder. There may be a small amount of reconstituted vaccine remaining in the vial after the 0.5 ml is withdrawn.',1,1),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="120">
+        <v>(10,'Men-C-ACYW135','The vaccine contains no adjuvant, preservatives, or thimerosal','Men-C-ACYW-135-CRM contains capsular polysaccharides from serogroups A (10 μg), C (5 μg), W135 (5 μg) and Y (5 μg). The vaccine contains no adjuvant, preservatives, or thimerosal. The container closures do not contain latex. The vaccine is packaged in two separate vials that are mixed prior to administration. Subsequently, 0.5 ml of the reconstituted solution is withdrawn from the vial that previously contained the meningococcal A powder. There may be a small amount of reconstituted vaccine remaining in the vial after the 0.5 ml is withdrawn.',1,1),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="120">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="E12" s="5">
         <v>2</v>
       </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" t="str">
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>(11,'HPV','HPV is the most common sexually transmitted infection (STI). HPV is a different virus than HIV and HSV (herpes). HPV is so common that nearly all sexually active men and women get it at some point in their lives. There are many different types of HPV. Some types can cause health problems including genital warts and cancers. But there are vaccines that can stop these health problems from happening.',2,1),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="75">
+        <v>(11,'HPV','HPV is the most common sexually transmitted infection','HPV is the most common sexually transmitted infection (STI). HPV is a different virus than HIV and HSV (herpes). HPV is so common that nearly all sexually active men and women get it at some point in their lives. There are many different types of HPV. Some types can cause health problems including genital warts and cancers. But there are vaccines that can stop these health problems from happening.',2,1),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="75">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
       <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" t="str">
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>(12,'Tdap','Tdap is a combination vaccine that protects against three potentially life-threatening bacterial diseases: tetanus, diphtheria, and pertussis (whooping cough). Td is a booster vaccine for tetanus and diphtheria. It does not protect against pertussis.',1,1),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="75">
+        <v>(12,'Tdap','Protects against three diseases: tetanus, diphtheria, and pertussis','Tdap is a combination vaccine that protects against three potentially life-threatening bacterial diseases: tetanus, diphtheria, and pertussis (whooping cough). Td is a booster vaccine for tetanus and diphtheria. It does not protect against pertussis.',1,1),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
       <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
         <v>0</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>(13,'Hib','Haemophilus influenzae type B vaccine is a vaccine used to prevent Haemophilus influenzae type b infection. In countries that include it as a routine vaccine, rates of severe Hib infections have decreased more than 90%',1,0),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="105">
+        <v>(13,'Hib','Prevent Haemophilus influenzae type b infection','Haemophilus influenzae type B vaccine is a vaccine used to prevent Haemophilus influenzae type b infection. In countries that include it as a routine vaccine, rates of severe Hib infections have decreased more than 90%',1,0),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
       <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
         <v>0</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>(14,'Pneu-P-23','Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. When you are immunized, you also help protect others because you are less likely to spread infection.',1,0),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="120">
+        <v>(14,'Pneu-P-23','Pneu-P-23 vaccine efficacy against IPD among the elderly','Pneumococcal infection can cause serious and sometimes fatal disease, including infections of the lungs (pneumonia), blood (bacteremia) and covering of the brain (meningitis). Meningitis can lead to permanent problems like deafness and brain damage. When you are immunized, you also help protect others because you are less likely to spread infection.',1,0),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="120">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="E16" s="5">
         <v>3</v>
       </c>
-      <c r="E16" s="5">
-        <v>1</v>
-      </c>
-      <c r="F16" t="str">
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>(15,'4CMenB','The 4CMenB vaccine is an immunogenic vaccine, though its effectiveness, impact on carriage and the duration of protection remains unknown. Further research, evaluation and surveillance will be required to determine the duration of protection, the efficacy or effectiveness of 4CMenB vaccine, its ability to induce herd protection, and the risk of adverse events with widespread use.',3,1),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="105">
+        <v>(15,'4CMenB','4CMenB antigens are important for meningococcal survival, function, or virulence','The 4CMenB vaccine is an immunogenic vaccine, though its effectiveness, impact on carriage and the duration of protection remains unknown. Further research, evaluation and surveillance will be required to determine the duration of protection, the efficacy or effectiveness of 4CMenB vaccine, its ability to induce herd protection, and the risk of adverse events with widespread use.',3,1),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="105">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="E17" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F17" s="5">
         <v>0</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>(16,'HA','Hepatitis A is an infection of the liver caused by a virus. Adults and children are equally at risk. The virus most frequently spreads through direct contact with infected people or indirectly through ingestion of contaminated foods or water. Symptoms include fever, fatigue, loss of appetite, nausea, vomiting, abdominal pain, and jaundice (yellow skin and eyes).',2,0),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="75.75" thickBot="1">
+        <v>(16,'HA','An infection of the liver caused by a virus','Hepatitis A is an infection of the liver caused by a virus. Adults and children are equally at risk. The virus most frequently spreads through direct contact with infected people or indirectly through ingestion of contaminated foods or water. Symptoms include fever, fatigue, loss of appetite, nausea, vomiting, abdominal pain, and jaundice (yellow skin and eyes).',2,0),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75.75" thickBot="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="E18" s="5">
         <v>3</v>
       </c>
-      <c r="E18" s="5">
+      <c r="F18" s="5">
         <v>0</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>(17,'Typh-I','Typhoid vaccine can prevent typhoid. There are two vaccines to prevent typhoid. One is an inactivated (killed) vaccine gotten as a shot, and the other is live, attenuated (weakened) vaccine, which is taken orally (by mouth).',3,0),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="90.75" thickBot="1">
+        <v>(17,'Typh-I','Typhoid vaccine can prevent typhoid','Typhoid vaccine can prevent typhoid. There are two vaccines to prevent typhoid. One is an inactivated (killed) vaccine gotten as a shot, and the other is live, attenuated (weakened) vaccine, which is taken orally (by mouth).',3,0),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="90.75" thickBot="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
       <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
         <v>0</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>(18,'BCG','Bacillus Calmette–Guérin (BCG) vaccine is a vaccine primarily used against tuberculosis. Tuberculosis (TB) is a potentially serious infectious disease that mainly affects your lungs. The bacteria that cause tuberculosis are spread from one person to another through tiny droplets released into the air via coughs and sneezes.',1,0),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>(18,'BCG','BCG vaccine is used against tuberculosis','Bacillus Calmette–Guérin (BCG) vaccine is a vaccine primarily used against tuberculosis. Tuberculosis (TB) is a potentially serious infectious disease that mainly affects your lungs. The bacteria that cause tuberculosis are spread from one person to another through tiny droplets released into the air via coughs and sneezes.',1,0),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:7">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add hospital location info
</commit_message>
<xml_diff>
--- a/database_draft.xlsx
+++ b/database_draft.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="加拿大健康安全新闻" sheetId="1" r:id="rId1"/>
     <sheet name="接种疫苗的相关知识" sheetId="2" r:id="rId2"/>
     <sheet name="疫苗信息" sheetId="3" r:id="rId3"/>
+    <sheet name="Thunder Bay" sheetId="4" r:id="rId4"/>
+    <sheet name="Mississauga" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="232">
   <si>
     <t>id</t>
   </si>
@@ -429,12 +431,401 @@
   <si>
     <t>Infections of the lungs, blood and covering of the brain</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Thunder Bay Regional Health Sciences Centre</t>
+  </si>
+  <si>
+    <t>980 Oliver Road</t>
+  </si>
+  <si>
+    <t>(807) 684-6000</t>
+  </si>
+  <si>
+    <t>The Dilico Family Health Team Clinic</t>
+  </si>
+  <si>
+    <t>200 Anemki Pl, Fort William First Nation</t>
+  </si>
+  <si>
+    <t>(807) 626-5200</t>
+  </si>
+  <si>
+    <t>George Jeffrey Children's Centre</t>
+  </si>
+  <si>
+    <t>200 Brock St E</t>
+  </si>
+  <si>
+    <t>(807) 623-4381</t>
+  </si>
+  <si>
+    <t>Centre For Addiction And Mental Health</t>
+  </si>
+  <si>
+    <t>St Jospeh's Hospital</t>
+  </si>
+  <si>
+    <t>(807) 343-2431</t>
+  </si>
+  <si>
+    <t>Residential Wellness</t>
+  </si>
+  <si>
+    <t>307 Euclid Ave</t>
+  </si>
+  <si>
+    <t>(807) 577-0519</t>
+  </si>
+  <si>
+    <t>Thunder Bay District Health Unit</t>
+  </si>
+  <si>
+    <t>999 Balmoral St</t>
+  </si>
+  <si>
+    <t>(807) 625-5900</t>
+  </si>
+  <si>
+    <t>Community Midwives of Thunder Bay</t>
+  </si>
+  <si>
+    <t>610 Hewitson St</t>
+  </si>
+  <si>
+    <t>(807) 622-2229</t>
+  </si>
+  <si>
+    <t>Primacy - Aurora Family Health Clinic</t>
+  </si>
+  <si>
+    <t>971 Carrick St</t>
+  </si>
+  <si>
+    <t>(807) 285-1894</t>
+  </si>
+  <si>
+    <t>Thunder Bay Veterinary Hospital</t>
+  </si>
+  <si>
+    <t>920 Carrick St</t>
+  </si>
+  <si>
+    <t>(807) 623-3531</t>
+  </si>
+  <si>
+    <t>Northwestern Veterinary Hospital</t>
+  </si>
+  <si>
+    <t>1160 Oliver Rd</t>
+  </si>
+  <si>
+    <t>(807) 345-3353</t>
+  </si>
+  <si>
+    <t>Elevate NWO</t>
+  </si>
+  <si>
+    <t>574 Memorial Avenue</t>
+  </si>
+  <si>
+    <t>(807) 345-1516</t>
+  </si>
+  <si>
+    <t>Crossfit Subzero</t>
+  </si>
+  <si>
+    <t>221 Bay St</t>
+  </si>
+  <si>
+    <t>(807) 252-1773</t>
+  </si>
+  <si>
+    <t>St Joseph's Hospital Audio</t>
+  </si>
+  <si>
+    <t>35 Algoma St S</t>
+  </si>
+  <si>
+    <t>(807) 343-2407</t>
+  </si>
+  <si>
+    <t>St. Joseph's Care Group</t>
+  </si>
+  <si>
+    <t>63 Carrie St</t>
+  </si>
+  <si>
+    <t>(807) 768-4441</t>
+  </si>
+  <si>
+    <t>CML HealthCare Ultrasound, X-ray, Bone Density, Mammography</t>
+  </si>
+  <si>
+    <t>194 North Court Street</t>
+  </si>
+  <si>
+    <t>(807) 346-6239</t>
+  </si>
+  <si>
+    <t>Mitomics Inc</t>
+  </si>
+  <si>
+    <t>290 Munro St</t>
+  </si>
+  <si>
+    <t>(807) 346-8100</t>
+  </si>
+  <si>
+    <t>Lakehead Psychiatric Hospital</t>
+  </si>
+  <si>
+    <t>580 Algoma St N</t>
+  </si>
+  <si>
+    <t>(807) 343-4300</t>
+  </si>
+  <si>
+    <t>Westmont Hospitality Group</t>
+  </si>
+  <si>
+    <t>5090 Explorer Dr</t>
+  </si>
+  <si>
+    <t>(905) 602-1137</t>
+  </si>
+  <si>
+    <t>Boston Scientific </t>
+  </si>
+  <si>
+    <t>6430 Vipond Dr</t>
+  </si>
+  <si>
+    <t>(905) 696-1800</t>
+  </si>
+  <si>
+    <t>Trillium Health Centre</t>
+  </si>
+  <si>
+    <t>5770 Hurontario St</t>
+  </si>
+  <si>
+    <t>(905) 755-0963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Trillium Health Partners</t>
+  </si>
+  <si>
+    <t>150 Sherway Dr</t>
+  </si>
+  <si>
+    <t>(416) 259-6671</t>
+  </si>
+  <si>
+    <t>Gt Hospitality Group</t>
+  </si>
+  <si>
+    <t>3939 Duke of York Blvd</t>
+  </si>
+  <si>
+    <t>(905) 363-7675</t>
+  </si>
+  <si>
+    <t>Veenarun Health Facility Ltd</t>
+  </si>
+  <si>
+    <t>3038 Hurontario St</t>
+  </si>
+  <si>
+    <t>(905) 803-0768</t>
+  </si>
+  <si>
+    <t>Mississauga Hospital </t>
+  </si>
+  <si>
+    <t>100 Queensway W</t>
+  </si>
+  <si>
+    <t>(905) 848-7100</t>
+  </si>
+  <si>
+    <t>Spinal Touch Wellness Centre</t>
+  </si>
+  <si>
+    <t>1100 Burnhamthorpe Rd W</t>
+  </si>
+  <si>
+    <t>(905) 232-8600</t>
+  </si>
+  <si>
+    <t>Erindale Animal Hospital</t>
+  </si>
+  <si>
+    <t>4040 Creditview Rd</t>
+  </si>
+  <si>
+    <t>(905) 232-8383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Credit Valley Health Center</t>
+  </si>
+  <si>
+    <t>16-2555 Erin Centre Blvd</t>
+  </si>
+  <si>
+    <t>(905) 828-0270</t>
+  </si>
+  <si>
+    <t>Pinewood Medical Centre</t>
+  </si>
+  <si>
+    <t>1471 Hurontario St</t>
+  </si>
+  <si>
+    <t>(905) 274-1475</t>
+  </si>
+  <si>
+    <t>City Centre Orthodontics</t>
+  </si>
+  <si>
+    <t>151 City Centre Dr</t>
+  </si>
+  <si>
+    <t>(905) 270-0888</t>
+  </si>
+  <si>
+    <t>Pediatrician Clinic</t>
+  </si>
+  <si>
+    <t>107-3885 Duke of York Blvd</t>
+  </si>
+  <si>
+    <t>(905) 366-4441</t>
+  </si>
+  <si>
+    <t>Mississauga Optometric Clinic</t>
+  </si>
+  <si>
+    <t>70-50 Burnhamthorpe Rd W</t>
+  </si>
+  <si>
+    <t>(289) 326-0707</t>
+  </si>
+  <si>
+    <t>Innomar Strategies Inc</t>
+  </si>
+  <si>
+    <t>55 City Centre Dr</t>
+  </si>
+  <si>
+    <t>(905) 897-0794</t>
+  </si>
+  <si>
+    <t>Living Arts Medical Centre</t>
+  </si>
+  <si>
+    <t>4100 Living Arts Dr</t>
+  </si>
+  <si>
+    <t>(905) 270-5600</t>
+  </si>
+  <si>
+    <t>Pediatric Urgent Care For Kids</t>
+  </si>
+  <si>
+    <t>4033 Hurontario St</t>
+  </si>
+  <si>
+    <t>(905) 270-5437</t>
+  </si>
+  <si>
+    <t>Membership Dental Clinic</t>
+  </si>
+  <si>
+    <t>3453 Palgrave Rd</t>
+  </si>
+  <si>
+    <t>(905) 270-3637</t>
+  </si>
+  <si>
+    <t>Square One Medical Management Corp</t>
+  </si>
+  <si>
+    <t>4175 Confederation Pky</t>
+  </si>
+  <si>
+    <t>(905) 848-4880</t>
+  </si>
+  <si>
+    <t>MyDiet Clinic</t>
+  </si>
+  <si>
+    <t>750-2 Robert Speck Pky</t>
+  </si>
+  <si>
+    <t>(647) 955-0461</t>
+  </si>
+  <si>
+    <t>Iona Dental Clinic</t>
+  </si>
+  <si>
+    <t>1585 Mississauga Valley Blvd</t>
+  </si>
+  <si>
+    <t>(289) 724-1708</t>
+  </si>
+  <si>
+    <t>Skinatomy Laser Clinic</t>
+  </si>
+  <si>
+    <t>4092 Confederation Pky</t>
+  </si>
+  <si>
+    <t>(905) 949-9198</t>
+  </si>
+  <si>
+    <t>NewLife Fertility Centre</t>
+  </si>
+  <si>
+    <t>4250 Sherwoodtowne Blvd</t>
+  </si>
+  <si>
+    <t>(905) 896-7200</t>
+  </si>
+  <si>
+    <t>Om Sai Physiotherapy Clinic </t>
+  </si>
+  <si>
+    <t>3960 Grand Park Dr</t>
+  </si>
+  <si>
+    <t>(905) 804-1117</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +862,13 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -509,7 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -553,6 +951,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1267,7 +1669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1826,4 +2228,941 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="17">
+        <v>48.424720000000001</v>
+      </c>
+      <c r="F2" s="17">
+        <v>-89.269339000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="17">
+        <v>48.354326</v>
+      </c>
+      <c r="F3" s="17">
+        <v>-89.256707000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="17">
+        <v>48.368693999999998</v>
+      </c>
+      <c r="F4" s="17">
+        <v>-89.269369999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="17">
+        <v>48.381236999999999</v>
+      </c>
+      <c r="F5" s="17">
+        <v>-89.246274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="17">
+        <v>48.380431000000002</v>
+      </c>
+      <c r="F6" s="17">
+        <v>-89.281597000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="17">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="17">
+        <v>48.400950000000002</v>
+      </c>
+      <c r="F7" s="17">
+        <v>-89.255039999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="17">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="17">
+        <v>48.405527999999997</v>
+      </c>
+      <c r="F8" s="17">
+        <v>-89.246095999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="17">
+        <v>48.407569000000002</v>
+      </c>
+      <c r="F9" s="17">
+        <v>-89.239671999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="17">
+        <v>48.412287999999997</v>
+      </c>
+      <c r="F10" s="17">
+        <v>-89.246420000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="17">
+        <v>48.42033</v>
+      </c>
+      <c r="F11" s="17">
+        <v>-89.272115999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="17">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="17">
+        <v>48.419418</v>
+      </c>
+      <c r="F12" s="17">
+        <v>-89.236067000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="17">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="17">
+        <v>48.429898999999999</v>
+      </c>
+      <c r="F13" s="17">
+        <v>-89.222678000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="17">
+        <v>48.439466000000003</v>
+      </c>
+      <c r="F14" s="17">
+        <v>-89.224908999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="17">
+        <v>14</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="17">
+        <v>48.444248000000002</v>
+      </c>
+      <c r="F15" s="17">
+        <v>-89.241731999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="17">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E16" s="17">
+        <v>48.444817999999998</v>
+      </c>
+      <c r="F16" s="17">
+        <v>-89.215982999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="17">
+        <v>48.449916999999999</v>
+      </c>
+      <c r="F17" s="17">
+        <v>-89.205640000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="17">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="17">
+        <v>48.457796999999999</v>
+      </c>
+      <c r="F18" s="17">
+        <v>-89.200532999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="tel:8076846000"/>
+    <hyperlink ref="D4" r:id="rId2" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D5" r:id="rId3" display="javascript:void(0)"/>
+    <hyperlink ref="D6" r:id="rId4" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D7" r:id="rId5" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D8" r:id="rId6" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D9" r:id="rId7" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D10" r:id="rId8" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D11" r:id="rId9" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D12" r:id="rId10" display="javascript:void(0)"/>
+    <hyperlink ref="D13" r:id="rId11" display="javascript:void(0)"/>
+    <hyperlink ref="D14" r:id="rId12" display="javascript:void(0)"/>
+    <hyperlink ref="D15" r:id="rId13" display="javascript:void(0)"/>
+    <hyperlink ref="D16" r:id="rId14" display="javascript:void(0)"/>
+    <hyperlink ref="D17" r:id="rId15" display="javascript:void(0)"/>
+    <hyperlink ref="D18" r:id="rId16" display="javascript:void(0)"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43.661169999999998</v>
+      </c>
+      <c r="F2" s="4">
+        <v>-79.596259000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="4">
+        <v>43.659393000000001</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-79.663528999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43.621172999999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-79.674308999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43.572477999999997</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-79.608740999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43.588369</v>
+      </c>
+      <c r="F6" s="4">
+        <v>-79.640973000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43.581254000000001</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-79.618127000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43.571568999999997</v>
+      </c>
+      <c r="F8" s="4">
+        <v>-79.608356999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43.569892000000003</v>
+      </c>
+      <c r="F9" s="4">
+        <v>-79.661198999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43.568455999999998</v>
+      </c>
+      <c r="F10" s="4">
+        <v>-79.665504999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43.562894</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-79.710297999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="4">
+        <v>43.564978000000004</v>
+      </c>
+      <c r="F12" s="4">
+        <v>-79.593965999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" s="4">
+        <v>43.590969000000001</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-79.639932000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="4">
+        <v>43.587530000000001</v>
+      </c>
+      <c r="F14" s="4">
+        <v>-79.639881000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" s="4">
+        <v>43.591847999999999</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-79.636275999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" s="4">
+        <v>43.593825000000002</v>
+      </c>
+      <c r="F16" s="4">
+        <v>-79.638249000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" s="4">
+        <v>43.588500000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-79.645640999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18" s="4">
+        <v>43.595061999999999</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-79.635784999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="4">
+        <v>43.585231</v>
+      </c>
+      <c r="F19" s="4">
+        <v>-79.633515000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="4">
+        <v>43.588968999999999</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-79.649420000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E21" s="4">
+        <v>43.596569000000002</v>
+      </c>
+      <c r="F21" s="4">
+        <v>-79.637106000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" s="4">
+        <v>43.592593999999998</v>
+      </c>
+      <c r="F22" s="4">
+        <v>-79.626467000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E23" s="4">
+        <v>43.589506999999998</v>
+      </c>
+      <c r="F23" s="4">
+        <v>-79.650722999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E24" s="4">
+        <v>43.600470000000001</v>
+      </c>
+      <c r="F24" s="4">
+        <v>-79.640253000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="4">
+        <v>43.580896000000003</v>
+      </c>
+      <c r="F25" s="4">
+        <v>-79.647699000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" tooltip="See detailed information for Boston Scientific" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Boston-Scientific/6992083.html?what=Hospitals+%26+Medical+Centres&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B5" r:id="rId2" tooltip="See detailed information for Trillium Health Centre" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Trillium-Health-Centre/6952062.html?what=Hospitals+%26+Medical+Centres&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B6" r:id="rId3" tooltip="See detailed information for Gt Hospitality Group" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Gt-Hospitality-Group/6976006.html?what=Hospitals+%26+Medical+Centres&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B7" r:id="rId4" tooltip="See detailed information for Veenarun Health Facility Ltd" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Veenarun-Health-Facility-Ltd/6930450.html?what=Hospitals+%26+Medical+Centres&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B8" r:id="rId5" tooltip="See detailed information for Mississauga Hospital" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Mississauga-Hospital/100360129.html?what=Hospitals+%26+Medical+Centres&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B14" r:id="rId6" tooltip="See detailed information for Pediatrician Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Pediatrician-Clinic/7798714.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B18" r:id="rId7" tooltip="See detailed information for Pediatric Urgent Care For Kids" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Pediatric-Urgent-Care-For-Kids/100513174.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B19" r:id="rId8" tooltip="See detailed information for Membership Dental Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Membership-Dental-Clinic/6945110.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B21" r:id="rId9" tooltip="See detailed information for MyDiet Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/MyDiet-Clinic/8080037.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B23" r:id="rId10" tooltip="See detailed information for Skinatomy Laser Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Skinatomy-Laser-Clinic/100365514.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B24" r:id="rId11" tooltip="See detailed information for NewLife Fertility Centre" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/NewLife-Fertility-Centre/2432353.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="B25" r:id="rId12" tooltip="See detailed information for Om Sai Physiotherapy Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Om-Sai-Physiotherapy-Clinic/3945499.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new location info in thunder bay
</commit_message>
<xml_diff>
--- a/database_draft.xlsx
+++ b/database_draft.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="232">
   <si>
     <t>id</t>
   </si>
@@ -1669,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2235,7 +2235,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2632,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2646,9 +2646,10 @@
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -2668,7 +2669,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2687,8 +2688,12 @@
       <c r="F2" s="4">
         <v>-79.596259000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="str">
+        <f>CONCATENATE("(",A2,",'",B2,"','",C2,"','",D2,"',",E2,",",F2,")",",")</f>
+        <v>(1,'Westmont Hospitality Group','5090 Explorer Dr','(905) 602-1137',43.66117,-79.596259),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2707,8 +2712,12 @@
       <c r="F3" s="4">
         <v>-79.663528999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G42" si="0">CONCATENATE("(",A3,",'",B3,"','",C3,"','",D3,"',",E3,",",F3,")",",")</f>
+        <v>(2,'Boston Scientific ','6430 Vipond Dr','(905) 696-1800',43.659393,-79.663529),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2727,8 +2736,12 @@
       <c r="F4" s="4">
         <v>-79.674308999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'Trillium Health Centre','5770 Hurontario St','(905) 755-0963',43.621173,-79.674309),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2747,8 +2760,13 @@
       <c r="F5" s="4">
         <v>-79.608740999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,'
+Trillium Health Partners','150 Sherway Dr','(416) 259-6671',43.572478,-79.608741),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2767,8 +2785,12 @@
       <c r="F6" s="4">
         <v>-79.640973000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,'Gt Hospitality Group','3939 Duke of York Blvd','(905) 363-7675',43.588369,-79.640973),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2787,8 +2809,12 @@
       <c r="F7" s="4">
         <v>-79.618127000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,'Veenarun Health Facility Ltd','3038 Hurontario St','(905) 803-0768',43.581254,-79.618127),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2807,8 +2833,12 @@
       <c r="F8" s="4">
         <v>-79.608356999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,'Mississauga Hospital ','100 Queensway W','(905) 848-7100',43.571569,-79.608357),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2827,8 +2857,12 @@
       <c r="F9" s="4">
         <v>-79.661198999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,'Spinal Touch Wellness Centre','1100 Burnhamthorpe Rd W','(905) 232-8600',43.569892,-79.661199),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2847,8 +2881,12 @@
       <c r="F10" s="4">
         <v>-79.665504999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,'Erindale Animal Hospital','4040 Creditview Rd','(905) 232-8383',43.568456,-79.665505),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2867,8 +2905,13 @@
       <c r="F11" s="4">
         <v>-79.710297999999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,'
+Credit Valley Health Center','16-2555 Erin Centre Blvd','(905) 828-0270',43.562894,-79.710298),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2887,8 +2930,12 @@
       <c r="F12" s="4">
         <v>-79.593965999999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,'Pinewood Medical Centre','1471 Hurontario St','(905) 274-1475',43.564978,-79.593966),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2907,8 +2954,12 @@
       <c r="F13" s="4">
         <v>-79.639932000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,'City Centre Orthodontics','151 City Centre Dr','(905) 270-0888',43.590969,-79.639932),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2927,8 +2978,12 @@
       <c r="F14" s="4">
         <v>-79.639881000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,'Pediatrician Clinic','107-3885 Duke of York Blvd','(905) 366-4441',43.58753,-79.639881),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2947,8 +3002,12 @@
       <c r="F15" s="4">
         <v>-79.636275999999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,'Mississauga Optometric Clinic','70-50 Burnhamthorpe Rd W','(289) 326-0707',43.591848,-79.636276),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2967,8 +3026,12 @@
       <c r="F16" s="4">
         <v>-79.638249000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,'Innomar Strategies Inc','55 City Centre Dr','(905) 897-0794',43.593825,-79.638249),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2987,8 +3050,12 @@
       <c r="F17" s="4">
         <v>-79.645640999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,'Living Arts Medical Centre','4100 Living Arts Dr','(905) 270-5600',43.5885,-79.645641),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3007,8 +3074,12 @@
       <c r="F18" s="4">
         <v>-79.635784999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,'Pediatric Urgent Care For Kids','4033 Hurontario St','(905) 270-5437',43.595062,-79.635785),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3027,8 +3098,12 @@
       <c r="F19" s="4">
         <v>-79.633515000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,'Membership Dental Clinic','3453 Palgrave Rd','(905) 270-3637',43.585231,-79.633515),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3047,8 +3122,12 @@
       <c r="F20" s="4">
         <v>-79.649420000000006</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,'Square One Medical Management Corp','4175 Confederation Pky','(905) 848-4880',43.588969,-79.64942),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3067,8 +3146,12 @@
       <c r="F21" s="4">
         <v>-79.637106000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,'MyDiet Clinic','750-2 Robert Speck Pky','(647) 955-0461',43.596569,-79.637106),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3087,8 +3170,12 @@
       <c r="F22" s="4">
         <v>-79.626467000000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,'Iona Dental Clinic','1585 Mississauga Valley Blvd','(289) 724-1708',43.592594,-79.626467),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3107,8 +3194,12 @@
       <c r="F23" s="4">
         <v>-79.650722999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,'Skinatomy Laser Clinic','4092 Confederation Pky','(905) 949-9198',43.589507,-79.650723),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3127,8 +3218,12 @@
       <c r="F24" s="4">
         <v>-79.640253000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,'NewLife Fertility Centre','4250 Sherwoodtowne Blvd','(905) 896-7200',43.60047,-79.640253),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3146,6 +3241,418 @@
       </c>
       <c r="F25" s="4">
         <v>-79.647699000000003</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,'Om Sai Physiotherapy Clinic ','3960 Grand Park Dr','(905) 804-1117',43.580896,-79.647699),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="17">
+        <v>48.424720000000001</v>
+      </c>
+      <c r="F26" s="17">
+        <v>-89.269339000000002</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>(25,'Thunder Bay Regional Health Sciences Centre','980 Oliver Road','(807) 684-6000',48.42472,-89.269339),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="17">
+        <v>48.354326</v>
+      </c>
+      <c r="F27" s="17">
+        <v>-89.256707000000006</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>(26,'The Dilico Family Health Team Clinic','200 Anemki Pl, Fort William First Nation','(807) 626-5200',48.354326,-89.256707),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="17">
+        <v>48.368693999999998</v>
+      </c>
+      <c r="F28" s="17">
+        <v>-89.269369999999995</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>(27,'George Jeffrey Children's Centre','200 Brock St E','(807) 623-4381',48.368694,-89.26937),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="17">
+        <v>48.381236999999999</v>
+      </c>
+      <c r="F29" s="17">
+        <v>-89.246274</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>(28,'Centre For Addiction And Mental Health','St Jospeh's Hospital','(807) 343-2431',48.381237,-89.246274),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="17">
+        <v>48.380431000000002</v>
+      </c>
+      <c r="F30" s="17">
+        <v>-89.281597000000005</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>(29,'Residential Wellness','307 Euclid Ave','(807) 577-0519',48.380431,-89.281597),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="17">
+        <v>48.400950000000002</v>
+      </c>
+      <c r="F31" s="17">
+        <v>-89.255039999999994</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>(30,'Thunder Bay District Health Unit','999 Balmoral St','(807) 625-5900',48.40095,-89.25504),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="17">
+        <v>48.405527999999997</v>
+      </c>
+      <c r="F32" s="17">
+        <v>-89.246095999999994</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>(31,'Community Midwives of Thunder Bay','610 Hewitson St','(807) 622-2229',48.405528,-89.246096),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="17">
+        <v>48.407569000000002</v>
+      </c>
+      <c r="F33" s="17">
+        <v>-89.239671999999999</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>(32,'Primacy - Aurora Family Health Clinic','971 Carrick St','(807) 285-1894',48.407569,-89.239672),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="17">
+        <v>48.412287999999997</v>
+      </c>
+      <c r="F34" s="17">
+        <v>-89.246420000000001</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>(33,'Thunder Bay Veterinary Hospital','920 Carrick St','(807) 623-3531',48.412288,-89.24642),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="17">
+        <v>48.42033</v>
+      </c>
+      <c r="F35" s="17">
+        <v>-89.272115999999997</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>(34,'Northwestern Veterinary Hospital','1160 Oliver Rd','(807) 345-3353',48.42033,-89.272116),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="17">
+        <v>48.419418</v>
+      </c>
+      <c r="F36" s="17">
+        <v>-89.236067000000006</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>(35,'Elevate NWO','574 Memorial Avenue','(807) 345-1516',48.419418,-89.236067),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="17">
+        <v>48.429898999999999</v>
+      </c>
+      <c r="F37" s="17">
+        <v>-89.222678000000002</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>(36,'Crossfit Subzero','221 Bay St','(807) 252-1773',48.429899,-89.222678),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="17">
+        <v>48.439466000000003</v>
+      </c>
+      <c r="F38" s="17">
+        <v>-89.224908999999997</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>(37,'St Joseph's Hospital Audio','35 Algoma St S','(807) 343-2407',48.439466,-89.224909),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" s="17">
+        <v>48.444248000000002</v>
+      </c>
+      <c r="F39" s="17">
+        <v>-89.241731999999999</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>(38,'St. Joseph's Care Group','63 Carrie St','(807) 768-4441',48.444248,-89.241732),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E40" s="17">
+        <v>48.444817999999998</v>
+      </c>
+      <c r="F40" s="17">
+        <v>-89.215982999999994</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>(39,'CML HealthCare Ultrasound, X-ray, Bone Density, Mammography','194 North Court Street','(807) 346-6239',48.444818,-89.215983),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="17">
+        <v>48.449916999999999</v>
+      </c>
+      <c r="F41" s="17">
+        <v>-89.205640000000002</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>(40,'Mitomics Inc','290 Munro St','(807) 346-8100',48.449917,-89.20564),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="17">
+        <v>48.457796999999999</v>
+      </c>
+      <c r="F42" s="17">
+        <v>-89.200532999999993</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>(41,'Lakehead Psychiatric Hospital','580 Algoma St N','(807) 343-4300',48.457797,-89.200533),</v>
       </c>
     </row>
   </sheetData>
@@ -3162,6 +3669,22 @@
     <hyperlink ref="B23" r:id="rId10" tooltip="See detailed information for Skinatomy Laser Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Skinatomy-Laser-Clinic/100365514.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
     <hyperlink ref="B24" r:id="rId11" tooltip="See detailed information for NewLife Fertility Centre" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/NewLife-Fertility-Centre/2432353.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
     <hyperlink ref="B25" r:id="rId12" tooltip="See detailed information for Om Sai Physiotherapy Clinic" display="http://www.yellowpages.ca/bus/Ontario/Mississauga/Om-Sai-Physiotherapy-Clinic/3945499.html?what=Clinic&amp;where=Mississauga+ON&amp;useContext=true"/>
+    <hyperlink ref="D26" r:id="rId13" display="tel:8076846000"/>
+    <hyperlink ref="D28" r:id="rId14" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D29" r:id="rId15" display="javascript:void(0)"/>
+    <hyperlink ref="D30" r:id="rId16" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D31" r:id="rId17" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D32" r:id="rId18" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D33" r:id="rId19" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D34" r:id="rId20" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D35" r:id="rId21" tooltip="Call via Hangouts" display="javascript:void(0)"/>
+    <hyperlink ref="D36" r:id="rId22" display="javascript:void(0)"/>
+    <hyperlink ref="D37" r:id="rId23" display="javascript:void(0)"/>
+    <hyperlink ref="D38" r:id="rId24" display="javascript:void(0)"/>
+    <hyperlink ref="D39" r:id="rId25" display="javascript:void(0)"/>
+    <hyperlink ref="D40" r:id="rId26" display="javascript:void(0)"/>
+    <hyperlink ref="D41" r:id="rId27" display="javascript:void(0)"/>
+    <hyperlink ref="D42" r:id="rId28" display="javascript:void(0)"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>